<commit_message>
更新tabletool v2 && storyeditor v2
</commit_message>
<xml_diff>
--- a/FirCehua/DataTable/ObjectPool.xlsx
+++ b/FirCehua/DataTable/ObjectPool.xlsx
@@ -1,75 +1,70 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
-    <sheet name="Client" sheetId="1" r:id="rId1"/>
-    <sheet name="Server" sheetId="2" r:id="rId2"/>
+    <sheet name="sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="11">
+  <si>
+    <t>name</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>min</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>初始化个数</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>对象名</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>索引</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>最大个数</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>int</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>string</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
   <si>
     <t>id</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>name</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>string</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>int</t>
+    <t>max</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>武器1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>索引</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>min</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>初始化个数</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>max</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>最大个数</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>int</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>对象名</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -85,11 +80,43 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="微软雅黑"/>
+      <family val="2"/>
+      <charset val="134"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="宋体"/>
+      <name val="微软雅黑"/>
       <family val="2"/>
-      <scheme val="minor"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="微软雅黑"/>
+      <family val="2"/>
+      <charset val="134"/>
     </font>
   </fonts>
   <fills count="5">
@@ -101,23 +128,22 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
-        <bgColor indexed="64"/>
+        <fgColor rgb="FFF2F2F2"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF00B0F0"/>
-        <bgColor indexed="64"/>
+        <fgColor theme="4"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor rgb="FF7030A0"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -127,37 +153,206 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF7F7F7F"/>
       </left>
       <right style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF7F7F7F"/>
       </right>
       <top style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF7F7F7F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
-    <cellStyle name="注释" xfId="1" builtinId="10"/>
+    <cellStyle name="计算" xfId="1" builtinId="22"/>
+    <cellStyle name="着色 1" xfId="2" builtinId="29"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="8">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <name val="微软雅黑"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FF7030A0"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color rgb="FF7F7F7F"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF7F7F7F"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="微软雅黑"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="微软雅黑"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="微软雅黑"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="微软雅黑"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="微软雅黑"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color rgb="FF7F7F7F"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color rgb="FF7F7F7F"/>
+        </top>
+      </border>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -170,8 +365,21 @@
 </styleSheet>
 </file>
 
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A4:D5" totalsRowShown="0" headerRowDxfId="0" dataDxfId="1" headerRowBorderDxfId="6" tableBorderDxfId="7" headerRowCellStyle="计算">
+  <autoFilter ref="A4:D5"/>
+  <tableColumns count="4">
+    <tableColumn id="1" name="id" dataDxfId="5"/>
+    <tableColumn id="2" name="name" dataDxfId="4"/>
+    <tableColumn id="3" name="min" dataDxfId="3"/>
+    <tableColumn id="4" name="max" dataDxfId="2"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -213,7 +421,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -245,9 +453,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -279,6 +488,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -454,73 +664,81 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="18.125" customWidth="1"/>
-    <col min="3" max="3" width="25.125" customWidth="1"/>
-    <col min="4" max="4" width="15.625" customWidth="1"/>
+    <col min="1" max="1" width="9" style="2"/>
+    <col min="2" max="2" width="18.125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="25.125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="15.625" style="2" customWidth="1"/>
+    <col min="5" max="16384" width="9" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:4" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C1" s="3" t="s">
+    </row>
+    <row r="2" spans="1:4" ht="17.25" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="C2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" s="3"/>
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D4" s="4" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
-      <c r="A2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D2" s="1" t="s">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" s="2">
+        <v>1</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="3" spans="1:4">
-      <c r="A3" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" s="2" t="s">
+      <c r="C5" s="2">
         <v>1</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="A4">
-        <v>1</v>
-      </c>
-      <c r="B4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C4">
-        <v>1</v>
-      </c>
-      <c r="D4">
+      <c r="D5" s="2">
         <v>10</v>
       </c>
     </row>
@@ -528,82 +746,8 @@
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D4"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
-  <cols>
-    <col min="1" max="1" width="11.375" customWidth="1"/>
-    <col min="2" max="2" width="12" customWidth="1"/>
-    <col min="3" max="3" width="17.625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4">
-      <c r="A1" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4">
-      <c r="A2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
-      <c r="A3" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="A4">
-        <v>1</v>
-      </c>
-      <c r="B4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C4">
-        <v>1</v>
-      </c>
-      <c r="D4">
-        <v>10</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>